<commit_message>
cory adding updated solutions file 2.5.A
</commit_message>
<xml_diff>
--- a/week-2/Solutions/2-5-A-data-validation-solutions.xlsx
+++ b/week-2/Solutions/2-5-A-data-validation-solutions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\data-analytics-lectures\week-2\Solutions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cory.jez\Documents\CJKB\thinkful\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF5D431-D39A-4DC5-9A27-90510F9CBBD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B14F3FA-C120-430C-B2A0-35A85A14989F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24090" yWindow="2940" windowWidth="21600" windowHeight="11355" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="starbucks-solution" sheetId="1" r:id="rId1"/>
@@ -380,7 +380,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
@@ -406,35 +406,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="8" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="8" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="8" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="2" applyBorder="1" applyProtection="1"/>
@@ -463,6 +434,50 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="4" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -810,35 +825,35 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" style="24" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="24" customWidth="1"/>
-    <col min="3" max="3" width="10" style="24" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="24" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="24"/>
-    <col min="6" max="6" width="25.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="24"/>
+    <col min="1" max="1" width="25.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -846,147 +861,147 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26">
+      <c r="B2" s="43">
         <v>2.95</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="43">
         <v>3.75</v>
       </c>
-      <c r="D2" s="27">
+      <c r="D2" s="44">
         <v>4.1500000000000004</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="46">
         <v>2.95</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="46">
         <v>3.65</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="47">
         <v>4.1500000000000004</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="2">
         <f>INDEX($A$1:$D$10,MATCH($G$1,$A$1:$A$10,0),MATCH($G$2,$A$1:$D$1,0))</f>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="43">
+        <v>3.75</v>
+      </c>
+      <c r="C4" s="43">
+        <v>3.95</v>
+      </c>
+      <c r="D4" s="44">
+        <v>4.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="46">
+        <v>3.25</v>
+      </c>
+      <c r="C5" s="46">
+        <v>3.95</v>
+      </c>
+      <c r="D5" s="47">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="43">
+        <v>3.45</v>
+      </c>
+      <c r="C6" s="43">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="D6" s="44">
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="46">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="26">
-        <v>3.75</v>
-      </c>
-      <c r="C4" s="26">
+      <c r="C7" s="46">
+        <v>2.4</v>
+      </c>
+      <c r="D7" s="47">
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="43">
         <v>3.95</v>
       </c>
-      <c r="D4" s="27">
-        <v>4.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="29">
-        <v>3.25</v>
-      </c>
-      <c r="C5" s="29">
-        <v>3.95</v>
-      </c>
-      <c r="D5" s="30">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="26">
-        <v>3.45</v>
-      </c>
-      <c r="C6" s="26">
-        <v>4.1500000000000004</v>
-      </c>
-      <c r="D6" s="27">
-        <v>4.55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="29">
-        <v>2</v>
-      </c>
-      <c r="C7" s="29">
-        <v>2.4</v>
-      </c>
-      <c r="D7" s="30">
+      <c r="C8" s="43">
+        <v>4.75</v>
+      </c>
+      <c r="D8" s="44">
+        <v>5.15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="46">
+        <v>2.25</v>
+      </c>
+      <c r="C9" s="46">
+        <v>2.5</v>
+      </c>
+      <c r="D9" s="47">
         <v>2.75</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="26">
-        <v>3.95</v>
-      </c>
-      <c r="C8" s="26">
-        <v>4.75</v>
-      </c>
-      <c r="D8" s="27">
-        <v>5.15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="29">
-        <v>2.25</v>
-      </c>
-      <c r="C9" s="29">
-        <v>2.5</v>
-      </c>
-      <c r="D9" s="30">
-        <v>2.75</v>
-      </c>
-    </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="49">
         <v>1.75</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="49">
         <v>1.95</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="50">
         <v>2.0499999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$2:$A$10</formula1>
@@ -1387,396 +1402,396 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" style="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" style="34" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="34" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="34" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="34" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="8.85546875" style="34"/>
-    <col min="10" max="10" width="13.28515625" style="34" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="34"/>
+    <col min="1" max="1" width="30.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="21" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="21" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="8.85546875" style="21"/>
+    <col min="10" max="10" width="13.28515625" style="21" customWidth="1"/>
+    <col min="11" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="34" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="22" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="38" t="s">
+      <c r="E4" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="G4" s="21" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="39">
+      <c r="B5" s="26">
         <f t="shared" ref="B5:B10" si="0">SUMIF($C$4:$E$4,$B$1,C5:E5)</f>
         <v>12000</v>
       </c>
-      <c r="C5" s="46">
+      <c r="C5" s="33">
         <v>8000</v>
       </c>
-      <c r="D5" s="46">
+      <c r="D5" s="33">
         <v>10000</v>
       </c>
-      <c r="E5" s="46">
+      <c r="E5" s="33">
         <v>12000</v>
       </c>
-      <c r="G5" s="34" t="str">
+      <c r="G5" s="21" t="str">
         <f t="shared" ref="G5:G10" ca="1" si="1">_xlfn.FORMULATEXT(B5)</f>
         <v>=SUMIF($C$4:$E$4,$B$1,C5:E5)</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="40">
+      <c r="B6" s="27">
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
-      <c r="C6" s="48">
+      <c r="C6" s="35">
         <v>0.02</v>
       </c>
-      <c r="D6" s="48">
+      <c r="D6" s="35">
         <v>0.04</v>
       </c>
-      <c r="E6" s="48">
+      <c r="E6" s="35">
         <v>0.06</v>
       </c>
-      <c r="G6" s="34" t="str">
+      <c r="G6" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>=SUMIF($C$4:$E$4,$B$1,C6:E6)</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="41">
+      <c r="B7" s="28">
         <f t="shared" si="0"/>
         <v>7000000</v>
       </c>
-      <c r="C7" s="49">
+      <c r="C7" s="36">
         <v>9000000</v>
       </c>
-      <c r="D7" s="50">
+      <c r="D7" s="37">
         <v>8000000</v>
       </c>
-      <c r="E7" s="49">
+      <c r="E7" s="36">
         <v>7000000</v>
       </c>
-      <c r="G7" s="34" t="str">
+      <c r="G7" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>=SUMIF($C$4:$E$4,$B$1,C7:E7)</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="42">
+      <c r="B8" s="29">
         <f t="shared" si="0"/>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C8" s="51">
+      <c r="C8" s="38">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="D8" s="51">
+      <c r="D8" s="38">
         <v>0.03</v>
       </c>
-      <c r="E8" s="51">
+      <c r="E8" s="38">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="G8" s="34" t="str">
+      <c r="G8" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>=SUMIF($C$4:$E$4,$B$1,C8:E8)</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="41">
+      <c r="B9" s="28">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="C9" s="49">
+      <c r="C9" s="36">
         <v>75</v>
       </c>
-      <c r="D9" s="49">
+      <c r="D9" s="36">
         <v>50</v>
       </c>
-      <c r="E9" s="49">
+      <c r="E9" s="36">
         <v>25</v>
       </c>
-      <c r="G9" s="34" t="str">
+      <c r="G9" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>=SUMIF($C$4:$E$4,$B$1,C9:E9)</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="41">
+      <c r="B10" s="28">
         <f t="shared" si="0"/>
         <v>125000</v>
       </c>
-      <c r="C10" s="49">
+      <c r="C10" s="36">
         <v>175000</v>
       </c>
-      <c r="D10" s="49">
+      <c r="D10" s="36">
         <v>150000</v>
       </c>
-      <c r="E10" s="49">
+      <c r="E10" s="36">
         <v>125000</v>
       </c>
-      <c r="G10" s="34" t="str">
+      <c r="G10" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>=SUMIF($C$4:$E$4,$B$1,C10:E10)</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="34" t="s">
+      <c r="F12" s="21" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="46">
+      <c r="B14" s="33">
         <v>100000</v>
       </c>
-      <c r="C14" s="39">
+      <c r="C14" s="26">
         <f>B14*(1+$B$6)</f>
         <v>106000</v>
       </c>
-      <c r="D14" s="39">
+      <c r="D14" s="26">
         <f>C14*(1+$B$6)</f>
         <v>112360</v>
       </c>
-      <c r="E14" s="39">
+      <c r="E14" s="26">
         <f>D14*(1+$B$6)</f>
         <v>119101.6</v>
       </c>
-      <c r="F14" s="39">
+      <c r="F14" s="26">
         <f>E14*(1+$B$6)</f>
         <v>126247.69600000001</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="43">
+      <c r="B15" s="30">
         <f>ROUNDUP(B14/$B$5,0)</f>
         <v>9</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C15" s="30">
         <f>ROUNDUP(C14/$B$5,0)</f>
         <v>9</v>
       </c>
-      <c r="D15" s="43">
+      <c r="D15" s="30">
         <f>ROUNDUP(D14/$B$5,0)</f>
         <v>10</v>
       </c>
-      <c r="E15" s="43">
+      <c r="E15" s="30">
         <f>ROUNDUP(E14/$B$5,0)</f>
         <v>10</v>
       </c>
-      <c r="F15" s="43">
+      <c r="F15" s="30">
         <f>ROUNDUP(F14/$B$5,0)</f>
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="41">
+      <c r="B16" s="28">
         <f>B9</f>
         <v>25</v>
       </c>
-      <c r="C16" s="41">
+      <c r="C16" s="28">
         <f t="shared" ref="C16:F17" si="2">B16*(1+$B$8)</f>
         <v>25.624999999999996</v>
       </c>
-      <c r="D16" s="41">
+      <c r="D16" s="28">
         <f t="shared" si="2"/>
         <v>26.265624999999993</v>
       </c>
-      <c r="E16" s="41">
+      <c r="E16" s="28">
         <f t="shared" si="2"/>
         <v>26.922265624999991</v>
       </c>
-      <c r="F16" s="41">
+      <c r="F16" s="28">
         <f t="shared" si="2"/>
         <v>27.59532226562499</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="41">
+      <c r="B17" s="28">
         <f>B10</f>
         <v>125000</v>
       </c>
-      <c r="C17" s="44">
+      <c r="C17" s="31">
         <f t="shared" si="2"/>
         <v>128124.99999999999</v>
       </c>
-      <c r="D17" s="44">
+      <c r="D17" s="31">
         <f t="shared" si="2"/>
         <v>131328.12499999997</v>
       </c>
-      <c r="E17" s="44">
+      <c r="E17" s="31">
         <f t="shared" si="2"/>
         <v>134611.32812499997</v>
       </c>
-      <c r="F17" s="44">
+      <c r="F17" s="31">
         <f t="shared" si="2"/>
         <v>137976.61132812497</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="41">
+      <c r="B19" s="28">
         <f>B7</f>
         <v>7000000</v>
       </c>
-      <c r="C19" s="41">
+      <c r="C19" s="28">
         <f>B19*(1+$B$8)</f>
         <v>7174999.9999999991</v>
       </c>
-      <c r="D19" s="41">
+      <c r="D19" s="28">
         <f>C19*(1+$B$8)</f>
         <v>7354374.9999999981</v>
       </c>
-      <c r="E19" s="41">
+      <c r="E19" s="28">
         <f>D19*(1+$B$8)</f>
         <v>7538234.3749999972</v>
       </c>
-      <c r="F19" s="41">
+      <c r="F19" s="28">
         <f>E19*(1+$B$8)</f>
         <v>7726690.2343749963</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="41">
+      <c r="B20" s="28">
         <f>B14*B16</f>
         <v>2500000</v>
       </c>
-      <c r="C20" s="41">
+      <c r="C20" s="28">
         <f>C14*C16</f>
         <v>2716249.9999999995</v>
       </c>
-      <c r="D20" s="41">
+      <c r="D20" s="28">
         <f>D14*D16</f>
         <v>2951205.6249999991</v>
       </c>
-      <c r="E20" s="41">
+      <c r="E20" s="28">
         <f>E14*E16</f>
         <v>3206484.9115624991</v>
       </c>
-      <c r="F20" s="41">
+      <c r="F20" s="28">
         <f>F14*F16</f>
         <v>3483845.8564126552</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="41">
+      <c r="B21" s="28">
         <f>B17*B15</f>
         <v>1125000</v>
       </c>
-      <c r="C21" s="41">
+      <c r="C21" s="28">
         <f>C17*C15</f>
         <v>1153124.9999999998</v>
       </c>
-      <c r="D21" s="41">
+      <c r="D21" s="28">
         <f>D17*D15</f>
         <v>1313281.2499999998</v>
       </c>
-      <c r="E21" s="41">
+      <c r="E21" s="28">
         <f>E17*E15</f>
         <v>1346113.2812499998</v>
       </c>
-      <c r="F21" s="41">
+      <c r="F21" s="28">
         <f>F17*F15</f>
         <v>1517742.7246093748</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="45">
+      <c r="B22" s="32">
         <f>SUM(B19:B21)</f>
         <v>10625000</v>
       </c>
-      <c r="C22" s="45">
+      <c r="C22" s="32">
         <f>SUM(C19:C21)</f>
         <v>11044374.999999998</v>
       </c>
-      <c r="D22" s="45">
+      <c r="D22" s="32">
         <f>SUM(D19:D21)</f>
         <v>11618861.874999996</v>
       </c>
-      <c r="E22" s="45">
+      <c r="E22" s="32">
         <f>SUM(E19:E21)</f>
         <v>12090832.567812497</v>
       </c>
-      <c r="F22" s="45">
+      <c r="F22" s="32">
         <f>SUM(F19:F21)</f>
         <v>12728278.815397026</v>
       </c>

</xml_diff>